<commit_message>
added upload to excel feature
</commit_message>
<xml_diff>
--- a/backend/sample_products.xlsx
+++ b/backend/sample_products.xlsx
@@ -1,44 +1,124 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d2a68cc714da4a1/Desktop/AlmaMate/Ecommerce/backend/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_4383411550397D6A206102AB8855B237A12C7E8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{568FCF32-6259-4F93-8C9E-ABB063D39B0D}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>sellerId</t>
+  </si>
+  <si>
+    <t>shopName</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>seller456</t>
+  </si>
+  <si>
+    <t>SportsWorld</t>
+  </si>
+  <si>
+    <t>Comfortable running shoes</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>seller789</t>
+  </si>
+  <si>
+    <t>FashionHub</t>
+  </si>
+  <si>
+    <t>100% cotton comfortable t-shirt</t>
+  </si>
+  <si>
+    <t>cotton-hoodie</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>nike</t>
+  </si>
+  <si>
+    <t>Oversized t-shirt</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxAQEhIQEhAQEBAVEBAQDxAOEA8NEA8QFhUWFhUVFhUYHSggGBolGxUVITEhJSkrLy4uFx8zODMsNygtLisBCgoKBQUFDgUFDisZExkrKysrKysrKysrKysrKysrKysrKysrKysrKysrKysrKysrKysrKysrKysrKysrKysrK//AABEIAOQA3QMBIgACEQEDEQH/xAAcAAABBAMBAAAAAAAAAAAAAAAAAQIDBAUHCAb/xABHEAABAwIDBAgCBQcKBwAAAAABAAIDBBESITEFQVFhBgcTIjJxgZFCsQgUocHRFSMkUmJyojVDU2N1grKz4fAWJTNEo8Lx/8QAFAEBAAAAAAAAAAAAAAAAAAAAAP/EABQRAQAAAAAAAAAAAAAAAAAAAAD/2gAMAwEAAhEDEQA/AN4oQhAIQhAIQhAIUTahheYw9hka1r3RhwL2scSGuLdQCQc+RUqAQo6idkbS972sY0Xc97gxrRxJOQT2uBAIIIIuCMwQgVCEIBCEIBCEIBCEIBCgq6yKEB0sscTS4NaZXtjBcdGguOZ5KZjgRcEEbiDcFAqEhNlHBUMfcse14BwuwODrHgbaHNBKhCEAhCEAhCEAhCEAhCr19ZHBG+aV4ZFGxz5Hu0a0C5KCl0j6QU1BEZqh+Bt8LGgYpJX2vhY3ecj5amwWlelfW3XVN46UfUodMQtJUuHN2jPJuf7S8t0w6VS7UrDUPu2Noc2mhJyhi+WM6uPHLQBYd4QLDXzxy/WBNM2e9zO2V4mJyzL74joN+a9TTdZ+12C314uG7tIadxHr2dz6leRSYAgy23ek9dX2FTVSzNBuGHDHEDx7NgDSeZF1f6M9N9o7Os2GfHCP+3qAZYgODc8TPJpA5LzjQnsO5B0D0J60qXaDmwSsNJVOyYx7g+KZ3COTLvfskA8Lr3648kNnDMjPUEgjmCNCugeqbp3+UIvq1Q4fXoW94nL6zEMhKP2tA4cc99gGwkIQgEIQgZNK1jXPe4NY1pc9ziGta0C5JJ0AC1D0v66GtLotnRdo7MGqqAWxDnHHq7zdbyIVPrw6alz/AMlQOs0OYa1zT4nZObD5AWc7nYbiFqSXVBd2ptWpq3mWpqJJ5DvkILWjg1vhaOQACip6ySHKOWWIcIZJIv8AC4KtEc0PQWp62WUWfLLKN4mkkl/xOKm2Ntiqon9pSzvgflcMsGOHBzD3XDkQVj4zmnThBurol1zxvwxbQj7F2Q+swAuhJ4vZm5nmMQ8ltilqY5WNkje2SN7Q5j43B7HtOhBGRC46DsvJbH6oempoqhtHM/8AQ53WZiOVPUOOThwa45EcSDl3rh0GhCEAhCEAhCEAtF9eHTHtpPybC68UTg6rcMw+cZtj8man9q29q2F1odMBsylJYR9bmxR0zTnhNu9KRwaCPMlo3rmZ7ibkkkkkuLiXFxJuSSdSTvQLTHvHyCsuKq0u/wA1YugRCbdF0DkhdZICmynJBJWaAqWir5aaaOphdgmjeHxuG48CN4IJBG8EhQzZsBTdQPJB1P0I6UxbUpWVDLNf4J4r3MMo1bzB1B3ghegXK/QHpW/ZVUJhd0D7R1UQ+OK/iA/XbmR6jeuoaKrjmjZNE9skb2tfG9pu1zSLghBOvN9P+lDNl0clQbGU/m6Zh+OZ3huP1Rm48mlejJXMXWn0t/KdY4sdelhxRU1vC/Pvy/3iBb9lreaDyL53SSF73F73SOke92Zc9xLnOPMkk+qllVVniCtSFAyn8Xolk1TabxFOl1QRg5qebRVic1Zk8KCAHUcQVJbE3zCr3+amiOXkSg6L6numBr6XsJXXq6YNZITrLFpHJzNhY8xfeFsBcmdE+kEmzauKrZchpwzRj+dhdbGzzsARzaF1XQVkc8cc0Tg+KRjZI3jRzHC4KCwhCEAoK+sjgjkmkcGRxsdJI4/CxoJJ9gp0hF8kHKPTPpJJtOqkqn3aw9ynjJv2UA8Lct5zJ5k7rLAvXQPTPqkpqrFNSYaSc3JYB+jSHmwf9M82+xWjukew6mhkMNTE6J+eG+bJGj4mPGTh5aXzsgx8ByVm+SqMOSsNOSBLpEgKLoHBMlOSUFMkKCdmcajiN2+Vwn0x7tlHFlcIEetr9R/TB8co2bJidFIXOp7AuMMnicLDRjszfcf3iRgehfVnV7RwyvvS0psRK9t5Jm/1TDuP6zsuAct59FOh9Hs1mGniwuIAkmf35pbfrP4chYckHluuzpaaOlFJE61RVBzSQbGKm0e7kXeEebjuXPAW++tLq1mrpXV1NKXzYGtdTTEBrmsFgIn/AAnU4TkSSbhaMr6OSF7opWPilYbPjkaWPaeYPz3oKrPEFZkOSqxnvKw85IG0upT5NVHSalPk1QQOOatv8Kpv19VbJ7qCoM7hSROy9VGw5pdPdBYc1bf6iOl2EnZczsjjloyTofFJF83j+/yWqdjbPqKqQQQRPmlOYZGLkDi4nJreZIC3V0F6pW00kdVVyY52ObJFDTucyKJ4IILn5OeQd2Q/eQbXQhCAQhCAWO25samrInQ1MTJYiDdrxm028TTq13MWKyKjqT3H/uu+SDjGI3A8lZj0UEQ7rf3R8lOzRA1IhNJQPamSJyZIgdE+wC9v1P0cNRtSNssbJGiGaRrZGhzRIzCWusciRmvEQi7PIr3HUibbWi5wVI/gv9yDpNrbJyEIBYDpX0Qo9pMwVEQLgCI5mWZNFf8AVfw5G4O8LPoQcv8AT/q8n2S5spkbNSvk7OOXJkjXkOcGPZxs12YyNt2i8i85Lfv0hf5Pp/7Qj/yKhaAkOSBaTUp8qjpNSpJEFd+qt/Cqb1aackFXevX9WfRiPalZ9Xle9kbYHzv7O2J4a+NuAE+G/aa23eq8e7VbQ+j4L7RmPCgl+2an/BBvLYOwKWhjEVNCyFmRIYO886YnuOb3cySVlEIQCEIQCEIQCr7RdaKU8IpD/CVYVLbjrU1QeEEx/gKDjuI90fuj5KduirReEeQVgaIGlMJTioygmTHpQUhQLSfEF7bqYP8Azen5sqR/4Xn7l4ekNnL2fVE7Dtmk5/WB708qDp1CEIBCEINXfSG/k+n/ALQj/wAioXP8ui6A+kN/J1P/AGhF/kVC5+lKBaXUqSQqOmTpUEL1ZboFVerDTkEFdy2r9Hdv6dUnhR295Y/wWqnarbX0c2/pVYeFNGPeT/RBvxCEIBCEIBCEIBYvpVJhoqxxyDaSpcScgLROKyibJGHAtcA5pBDmuAIcDkQQdQg4ujGQ8gpwcl1JU9XuyJHY3bPpbnM4YxGPZtgp6XoTsyLwUFGOZp4nH3Iug5RcRxHumMAPxN1DRmTcm9tByXUlTsWl7Z0TKehhDQDidTU93kgHe3mn7S2LEIo2OhpiXSgHBDGI3DdcAWPsg5ZBAtcgeZAQJG/rN9wuqNmbFioZGRsgpmskJv2EEUBxZZ90C+5ZTZTjI15dYkSOaO6BkALaIOQYSMV7iwzJuLAL2fVu7BtaieSLCZ7XebopG+uq3VtjZUNVTsknhp5bPcHGSGJzjphsbZb1Yn2IIBHhZTsHaAM7GGOLC7PPutCD1yFiKqonjEcZewyPce/YBrWi271S0tXI2URSPbIC0uDmgAi1zbLyP2IMshYekqp3gzlzRGA8iIAXdYG2dr6plHPPLZwnizOcdhcC/ug8Z9IB7Ts5jbjG2rgfhzvbDI3/ANlzzKeY9wuq9s7JFVMYpWQytw42tnjbLGACbXa4EXFzmoW9HqftHQw0lDGGNbc/VYBiJAv8HNBy5TlWoaKWXOOKWUcYYpJRfzaCumdq9DtmNBqHUFI+cBgJMTcJdk25YO6fZZalp6lgZYxuZleNrWxhjeVgEHJddRviyka+N2QLZY3xHMX+LyS00TpC1jGuke7wsjaZHuyvk1tyV1RM9jZKhrmCQvLWtjc0Pa456g7la2D0egpQXMggjkdm90MEMOu67Gi6Dk6t2bPFnJDNEOM0MsQ93ALan0cR+frT/U0493v/AAW9HRAggi4ORBzBVSg2PTQOe+GCGF77do6KKOJ0lr2xFoztc68UF5CEIBCEIBCEIBCEIBI5wGZyHNV62q7MEgXOWXrZYx1S5+ZPpuCAr65jnlrqZ0gGTZB8XqNFDHSSCOIYSfz4fhBxYGZa/apg6+qQxcx7ZoLG1j+cgIuQ1xLsOdh3deCrUM7ou0YInyAvc5pYL65Zjdog2GiaJSPuQPbs+Q0vZ4bPxYg02uRf8FLVtlmia7sy2RkgOA/FYaj3+xTU9cR4sxkL7x+KyIN0GG2hG+VsUphJwl2OInMi4/D7U6ghBcXCm7IBpwucSHYiLWt6rMIQYzZTXxwZsOMYiGHukm+WqoVEJlsGUzon4gcfgaF6JCDE1scjJmzNYZBgwOAyO9W6g9mDIyLG82Dg3Jx8zbcrMjw0EncsdJVl3IcEGNlY5wncW4XPLMLNT3Tc3O7RWqfa0jsDBFhtYPdJcNtvshzjx+5IG31+QQRvpmPknLja9uyfmbHjl5BX9lVpc3DILPBtc2tIOIKpubb/AOBOa4/6IM2hYyGrc3mOBV+GYPFx6jggkQhCAQhCAQhCAUc0oaLn05lSLG1M2I8hp+KCvUklpJ1JCqsVupGQHmVWAQPCEAJQEDU17clIQlY1A2AXBHIrIUNRoDofsP4FUKTUhPjyy9EGbQq9JNfI6j7QrCAQhQ1MlhbeUFarlviG4NNufNUotFZeO6fL71ViQPlGSGJajwpI0CvGSjgKntkoIfEglcMxzyS0suE/McQnOH3FQvFnFBmmm+aVVKKXd7fgraAQhCAQhI45IK1bNYYRqdeQVIIkcbm+qWNA2pGnkq9lbmGarEZoHWRZOsiyBpCdEM0hT4xmghjyeU8jM+abJk8FSzDPzCB0biMxqNFkoJQ4XHkRwKxjFLTYg+48Jydf5+aDIk2zWPlfiN1NWS/D6lVkDn+EqrGFbeO6VWYM0D6kd0JkWikqtAmR6IJgMlVj8SuNGSqN8SC3b7QoZRn6BTO3FNlHyQRxmyykT8QusQHWOat0k1jbigvoQhAIQhBDLAHKsIC08Qr6RwQYx4Vd4zVlxUEmqBbJbIS2QNKfGmlPiQQ1QzTnd7DbMqR4BJCkpmAOHqgdBTbyrjGAJwCVBBUU4d5qmYy05rJprmgoKL/D6hV2DNXKiOw9VWjGaAq9AmRaKSr0CZEgnZoqgHeVxiq2zQWnDJMB4qQaJIW3NkEZiL91lap6YNU7WgJyAQhCAQhCASFKkdogxSjdqpyFC7VA6ycAgJwCCJSRptk5qBs+TgeSmg8QUVZuPNS0+o/3uQZBCEIBCEIIKvT1VOMZq5V6eqqRIEq9yjjUtUo4wgnYqztVaYq7hmUFhqdD4vRNanw+L0QW0IQgEIQgEIQgE1+h8k5NfofJBj1CdVOQeCjMZ4FABSJBG7gnhpQREISlridEpjdwQFSLtSUZvh809zTa1lFSRuDtMroMqhAQgEIQghq9PVVYgrdSMlUjB4IEqUyIKScck1kTkEjVA4ZqwGkKIsJOiCRuikh19FGGOCkp9UFpCEIBCEIBCEIBCEIGlgRgCchA3CEuEJUIGhoS2SkpuMcR7hApaEBoTHzsBALmgk4WgkZmxNv4T7JPrDL4cbcW9uIX3bvUe4QSoUZnZe2Nt7E2xC9hYH5j3QJm3IxNuBd2YyGevsfZBIhM7RumIX01Gqjmq42GznBpsDY6m5sMuZQTEJMAVc7RhuR2jbgkEXzBG63H5pPynB/Ss1IycDcjW3FBZwBLZV4q+FxDWyscSbNAcCXZE5ccgfY8FZQJZAaEqECWQAlQgEIQgEIQgEIQgEIQgEIQgEIQgiqYGyNcxwu1wsbEtPoRmDzCo/8AD9L/AEQta1sT7WvfS/8AsZJEIHHYdOcILCQ1oa273nIBwFze5Pedmc+8eJSfkGntYsJGZOJznXJcHG9znm1vshCBXbCpz/N2u1rTZzhkMNtDr3G56nCE5uxoBmGkHCGZPf4Q7EBruOaEIEbsSnBxdn3sbJLlzjZ7Tdp1UtRs2KS+IGxYY8IcQ3CTiOWgJNs9ckIQMfseE4iWm7sV3Y34u8Gg2N7jJgHlcbzdXbIgJv2YxYi8OFw4PIAxA7j3RmhCAptkwxlpY0twm7e+8gGzxvP9ZIfNxV5CEAhCEAhCEAhCEAhCEH//2Q==</t>
+  </si>
+  <si>
+    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEhUSEBIVFRUSFRAVFRUVEBAVEBUVFRUWFhUVFRUYHSggGBolGxUVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OFxAQGisdHh0rLS0tLS0rLS0tLS0tKy0rLSsrMC0tLSstLS0tLSstKys3Ky0tKy0tKy01Ky0tLS0uLf/AABEIAOkA2AMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAEAQIDBQYACAf/xABFEAACAQIDBQUEBgkCBAcAAAABAgADEQQSIQUTMUFRBiJhcZEUUoGhIzJCkrHRBxUzU3KiweHwFmIkQ4LxY4OjssLS0//EABkBAQEBAQEBAAAAAAAAAAAAAAABAgMEBf/EACMRAQACAgICAwEBAQEAAAAAAAABEQISAxMhYQQxUTIikYH/2gAMAwEAAhEDEQA/ANsRGMJNaNZZlA7CRlYQVjGEoGIkZEIYSMrKiBlkZEIZZGVhlCVkbLJyI1hKByI0rJyI0rAgKxrCTERjCVEBEZaTFY0rCISI0rJisaRAgIjCJOVjSkCAiMKwjLGlJQORGmEFIwpKICI0iTFI1hAiiR5E6QfTcsaVk1o0icnZAyxhEnIjCIAzLGFYQyyNllSg7LIyIQVjCsqByIxhJykYVhEFo0rJysaVhAzCMYQhlkZWVEJWMtJyIwrKIisjKwjLGlYEGWNtJ8kTJCICkQpJykTLAHKRpSElY0rAFKyM04WyxppygJknQopEix9FtEKyS0Qzk7oiIwiTkRhEIgKxHElIjSsAZlkZWFFY0pCUFZJGUhbLI2WUClYxlhRWMKRaBCsYVhTU40pKlBckTJCTTiZISg2SNyQopEyS2UFyRMkL3c7dxZQPJGlIYacaacWBMsTJCTTiGlCBCkayS0oYFjrB6lLUiLWgBSdCXpzpUbkiNIkhES05uyMiNtJCsS0gjIjSsnyRhECG0YVk5WIVlQOVjCkJKxpWAMUjTThWWJkhAppRppQ3JEyQUC3UaaPhDwLRHN4spXmnENOFlIwpBQfdxMkIyRwUSpQQpG7m/CHWHSPD+EWtBBgTziJSAMJeoTICpkD3rgCwley3MLNONNOWEnyCanOhZpzpbSmntEtFiEzDqQiJaLOEBCI0iPiXgMKxuWc1QDjK6pt2kpsT+UllLC0QrOw9daguhBElyypSHLOyyXLOtKIwIhEktFywICsaUkqa3ilYA5WNKQkrEKQgUpEyQrdxN3BQbJOyRcXXWmt2Mz2M7Voo7mszOUQsRbQZImSZrB9r1ZgCLXnba7UogIXpJvC6y0mURrJPm+F7aMKwzG685d7c7Rd1Xpm3ONzRqyk6YfZ/b3vZaq6dZ0u0JrLY4TbLA9/hLmnj0ZcwYTCGtOp4i05xMw6TENidtUusbhdt02Njp5zFvWuY3fRtJUNxtbaYRO6bk8Jk6m2KpOrnjyg2Ir3HGV71JLmT6XL7QqPpmMEpspa1Q6QIYiw04yEVYotq9i7SSk2UaqeBmtSoCLgz5TvSDaF0ts1AMgcgSxlMExb6S9dRxIlVjNsgEin3rC58Ji22oeBYnzMrqGOy1AS3VgD9W57oNuGgzW85rG85pjOYwi30vYe0jXW5FiLy0tPnuC221G5pqcpYjMbfWsGYfzS5TtbTy9695r+fErFTFw06kASBsWl7ZhMdtLtOXFk0vM3UxjFiSxv5mZnJafUMTj0TUkWmX2j2wyVLKLqDqb8pmTjHYEZjbzlPXqd7WSJmSYh9jwu06ToHDC0qdr9pESwQ3JmM2dictM2JtKzF7QUecxOcz4hqMYWPaDb9RjYnQ9JkauPNzrFxlYnvSHDbPq1T3Kbk+Cn8TpNYx+kr7Y9YZC3MSt2rjbmabZnYzGlQLLTBt9Zrn0EucJ+janxxFQt4DuiSMfNlvlrV9eEsd87ILm4k23cNRo16lNaeiGw1MJ2Eu8DqlIEqARO08c1bnvF0oHFjEmsTZNVmH/DqBcXnSNbLmniBfWOqYgHgJbr2UqfvB6R/+lqn7wek47Y/rTPNVjDVmkXs1VH2lPwkLdlKp+2sb4pSiNTSDvUmlHZWr74iHslVP2x6S74/pTMBteB8gOMuamxqgA1TP+7zWe/TXQnwvJsZsarhAK6sHdWVaakd0u/dUnwW5c+CShr4mspzGo1WxuwyqPNqYtfToSbjxnbiwjkiZceTOcDsQ5F7ixFwQQQQRxBHWB7zneaRsMMWgrUrvewqBNWVhoCRxsf6Qd9iU0QvWY0kHFqhyL89SfAAzOlTTpGVxajNXXTW9gBzJJsABzMbj91TZRWcq4uDTprva3G4GUaL8TG4vaQW4wYampuDiHW2Ia/HdKf2S+J7xlFhq6IctMG4NywI10+0TqfhO2HHU24553FNXhdoKFzIAEqlKZTFU7VWKtoaIQ6sdRwtw42tGbSrJnqbgNkpFEqc1SoQe5m4cQbSnpkZs9u9yI4jW8vdj18jqpRXTEVDvktmJzJlUi3F+BvpbWazwtnDOvEK8YiRvXl1snZNGuq97I7VXpZGb7YuVUHU6qOfPnLI9j096efKsPt6Mf8AX0ylLF2BgdapebJuxq+9Iz2OX3pnsxXXJQ7KQ12WirZb85scL2Awy61qrP4FlVfQQTZ3ZlaVQODe0uK2HJmJzwtqpT09j4CivcVL8uBMBqbTAc5EAtblIX2c1xbreI2zXLMbjWN8f0qV5V2mcp8l5yy3+g8hMxVwFQiwPIfKWlmCjXgBHZj+lPlPadv+Kr/xS4/R3+1f+GS7R7JPVq1Km8AzHQWiYLslWpG6VspI5TvPNhrVuGk3bcW15Tpj27O4k8cQ3rOnLsw/XWpaw7fT3vxjP9Qp1PoZSCk3MKPScV6uo8p5+qP130lcntGvIMf+kzv9Rn3GlGWUfaJ8hF3y9CY64XrXn+oH5L84n68qe7KRcR7q/iTJ6e8PK3yjrhesfi8a7gO+SyllCFsrMzoR3DwzBc2njMzUxeHqG1QNRI4VEuyeG8p6keam3hLzEltyV7zA5s2QhyF0FmouuR143Ym4toDMZtRzpZVtysxKdABUIBp/w5LeM9/Fh/iIjw8HN4zv7WuJ2JWAFWlaspGlXDVXV2HiEYFvnKHE1EUlnDZ11JqtUZ16/tCSvykOF2lVw7lqLlGJ1W+jH/enA+cu6Xa2jiPo9o0F5WbLmp+ZH1h5i4HhMZZ83F5mN49ff/GsMOPk8ROs+/pkcVjWq6DROvNvLwjadlGk3rdk8FXXPQdlB506gdPirXt5XEqsV2Grr+zq03/iDUz/AFHznPD5/Dl4man26ZfD5I+ouPQHZuENajVenc1KNnZOOalzKga5ha9uYMTAY8qbq1j1B1146zXdj9gthc9Sq4NRwFst8qKDf6x4knwHCZbtls4UMRdNErAuByBBs4Hhcg/GOD5uOfNlxxN/hzfFnHjjOf8A0ZhsYpDLcLnUXa1zdGDIRaxBBGhB0vL/AGftxr5qiE08qKzZ/pcyk2Nr6kqdTblPnIxBH5czD8LtIg5TqTbQEX8dDae6Yxy+3kicsfMPpGz8cMRnFHMWpuylCLMUsCKgB1trbziVazDQ3HncH5zIbB2ytCozqt3qBb3Zlay+6COHw6TVL2ypsLVRe3J1DfOefP4t/wAvTh8yvGUGvim8Yz29vek361wlT7Fj/sYqeXLhHPg6DfUrFfB0DfMEfhOM/Gzj29GPyuKfvwH9veJ+smHONrbJbijo9hfukg+hgVfC1qf1lcXAI0uLHncTllxzH3DtjOGf8zY79aN734Rf1k/vCUrYkjofhGe0jmg9ZNI/CcIXYx7+HrGfrKry/ESm36cww8jFVkPCqw8/7x14s6QuP1pW/wAtOlUEb7NVT52ixpiaQuaOBLcFZvJT/WErslrd4Kn8Tj8BObEVX41Gt0BsPlGbi/HXzMlutSccPRX61W/giX+cY1WiPqUmbxc/0j/Z/CIaB6RZqhqYxz9VVUeCiDsHbQlifP8AKF2PSWnZ50p1C9QC9gEJFwDfU+fCXHzNJl/mJkNtrsrihRQCgtVlFwBVUshNz3VLAX114/GYTaeysWlzVw1YNzO4YK38S0xZvOfZnxqNz9DA6gJ+pVb4OZ9HGah8rLC5t8Hq5hpkdfAU2Hwva5HhIwHHClU52+jqH5kT7lUo1zwr/hf8DAq2HxP7/wDnt/SXY1fG8OcTTbPRWsjdUSrY+YtY/GajZvbSuumKw1RgPtpSqK3xUi011XDYnW9fTwqG8CZMUDYVr/8Anf0M8/NwcfL/AFFu/Hy58f8AMhk7cYHnVZT7rUaob5AzJdqNvLiqqlAQlNSq5hZjc3Ykcr2HpNhWSuwtVpJVHMPSpVB+F5XVNhYJ/wBphXonrQqun/p1Ay+lpy4Ph8XDntjdt8vyOTkx1lhSf8FifQi3xvOVracB7oIzMDxBV+HwM2x7FYYj6PFVl6b2gjD1Qj8Iwdgr8MZhz4MtRT6ET23Dy1LLUalhl4ZrdzMVGXplqXXzF+ULos1wLMPgQhUcPqkofQTR0+wNS91xOGN//FqW9LWk1H9H9ZdN9hVF76OePWwEsTDMxKpw1a3P+/naHU8ceRlph+wbMdcXT8clGq5/pLvA/o9ogg1KtZ/CyU1PmdT6TW8MdcyoKOM4a9OB+VucuNsYuqKGH4o/0wsRYlAVKmx5amXp9jwelOkmcfZXvP8A9TtwmX2tialeoaj+QHIDoJ5Pk8sTFQ93w+CYy2kONq30q0abjrls3qIzNg34ipSPh3lkTUT0EjNA9J5dnvnCBC7GV/2Nem/gTlb5wfE7Erpq1JrdVsw9RI3w/WS0cRWp/s6jjwBNvSW4TXJXPQsdQR5i06Xybfr8KiU6o/30xf1E6Vnz+CGrjkwsP84Rwrr715QE6crcNTr/AHi5XHPTkTyH+XmdS2hOKHWRCurH+8A2ds3EVjZBp7xuE9Tzl4Nk0KADYly7a2QWP8o1I85dGZzoPh6LVDakpbqdco+MsRgadEXxFW7H/l07lvIk/wBpX4nbtRu5TtSpgcAAGtz4cPhKxzz1bxGvxvzOsVEH+p+/CbbW0qKDPm3KggAavfoOt7dOEoV7e0gTcueFiFJHj9azD0Ml2pswVdb6i44aacbj+so8VsJk+sl/EC4nbjy9uPJx39NPT/SDQ51SR3vsVCdBcDiDrwjqnbvC/vG+FOv4dH8flMX7CL8BfynHCeX9Os67uXU0lftxh76CoTr/AMlyP5qkDbtlRJvun890P/0lL7N4ekU4cf4I2OtbjthRvpTqDxCEfg8tMH29oD62c+BRz/QzJ+y+E72URsdb6Lhu3mz2HeIXzDj/AOEJHbLZfv0/vN/9J8zGHEU4QX4CNzql9OHbLZX7ymPLMT/7R+Mhb9Jeyqf1N45F9FoW59WInzf2JOaj0EaNnU/cH3RG51S3GP8A0yqRbDYZhxuajqNOVgt5W0v0o1XP01MMt/qK7KvxI1P/AGmZGzKfuLF/VyclEk5W1jhMNxR7T4OuPo23L/u3B3ZboGHCMxW1lp/tFI6EaqfIzGexL0EsNnVwndqqXpniNL/C/ETjPFjLvHLnivP1xSPByPMSVNo0z9oecDq9maVdS+BqXPOk5sR4DmPjp4zOYrB1KTFKilWHJh/gPwk6oWOeWy9qT3gZzVE5H0mKVz4+slp4hhzk6m+5rM4nTOJjiJ0nXK9sNtgez9arqVCDjmb8pdYfYuGw6k1iHItx4eFkkGO287aU+6vM8/hATVzaklvE8YmYhzrKftYY3brHu0RkXrl73wHASrNG9yxuxNyT08T1hAcH4SSllN7+dusxMzLUYxH0HGDuMwXrcXuB5SWngx0sDflyhAraXtxOovGb8WNib34HWRpF7KCAR5fLjE9kXz5am/zjjXHAm34Rq1deMATE7KpOSCmo56g+olfW7N0zwYr/ADS73tuesbTrC/jLGUwawzT9nW1yuPiLQVth1R0PxmvaoLxVYdBNdmSaQxFTZtVeKGDNQYcVPpPoDWkNWkDyHpL2ynWwJXzjgs2NTAIeKj0g1XY6HhpNdkJPHLMCmZxUy9fYzcmgtTY1S+hE1vDOsq0qek4L1hx2VWH/AHjP1fVHBZdoSpCEHpF1hXslX3ZG2Hq+7FlSipV3QhkYqRzBsZpMJ2gpVlFLG0wR+8A+ZHEHxEzxo1Pcjd0/uGLZnG2i2h2PDDeYNw6EXsTr5A/nMtjMFUpHLUUqR1Gh8jLHZuNr0WvSJXqPsHzE2+zduYbEqKeLp5WOmouh+PKW2ayj2+XZTOn07bHYKk4zYRgvhe6H8osWtwqVqmS0q0rs5nJVM4U7WsxWkoraSq3seKhkpbWKVjfWPzjWVwqThVMUWMrYgGMSoIEX6zmqRS2PNbSRDEQQVY4GKNhK1TJFqwJqkZnil2WJriNOIgSvOapGpsOXFCJ7RK9XEXexqbDhWERqkA3k41Yoscaukj3kD3k7PLSbCTUjHeDmpE3kUlpzWjGqwdmjGaWi0lRxImaNZo1mlpLWWytuVqB7jXX3SdJ0qmedNM1Eikq6Ry1AeEBzxyvFFjgY8PAhVibySlHF4orwE1Ym8iixhqxC8D3kTexQN3kTemCbydvIosVvIm8g28ih4osSasTeQYvGl4osVnibyC72dvJaSxReJng4qRS8UWJzxDUg28nF4otOXjS8hNSNFSKLT5pxaQZ40vFFpWeRlpGWjS0tIczzpA7TpRKKo6j1Edvh1HrPTnstP3F+6v5TvZafuL91fym9HDu9PMRrjqPURN+Oo9Z6e9lp+4n3Vney0/cT7ixod3p5g9oHUeoi78dR6ienvZafuL91YypRpKCSiAAEnuLwGp5Rod3p5k3w6j1E7fDqPUT01QSk6q6qhVwrA5BqCLg6jpGE0LkfR3DKhFkuGYBlU+JBBt4xod3p5p346j1ETfjqPUT077PT9xPurGOlEFQVpgscqghbk2LWHjYE/CNDu9PMntC9R6id7QvUeonp72en7ifdWRUBRfNlVDlYoe4NGFrjh4iNDu9PM3tA6j1EacQOo9RPUBw9P3E+6s44en7ifdWNDu9PLu/HUeoimuOo9RPUPstP3E+4v5QGhjsK+fLk+jBZiaeVcouC6swAZQQRmFxpLodvp5rGIHUeojhiB1HqJ6VGKw2akncDVwTTUpZ2AXMTlIuBYc7SEbUweWoxamFpDM7NTKrluRmUsAHW4IutwTpxk0O7084HEDqPURPaR1HqJ6UfG4UMiHJeoEZfoiRZyQhZgtkzEEDMRcggcJGu08GQxGU5CoNqD3bMxVTTGW9QFgQCtwbGXQ7vTzf7SOo9RO346j1E9IjaWEugun0uXL9E2XvEqoZstkJYFQGsSQRxkuBxOGrFlphSUsSDSK6EkBlzKMykqwzC47p10jQ7vTzTvx1HqI04gdR6ieo/ZafuJ9xYvstP3E+4v5Rod3p5Z9oHvD1ETfr1HqJ6m9lp+4n3F/Kd7LT9xfuLGh3enlY1l6j1EWeqPZafuJ9xYsaHb6TTp06bcXTp06B0pNt7KqValN6eUZFqKSzmwDcQKeQgnT62ZSPHhLuJAylPs5Wpbs0TT+jWmCheoqM24ek7Zgp1uynhrbW3GMpdl6i37lFzvMLUuzuCxpUkpOh7hsLqWB1ve1hxmunCBk8N2YqAgVCrDeo7MarneqpqEl6eQBW745te3HQR1Ps3UDK1qVkrtUVWqMzAMlRWbebsEkF1YKQfq2zdNVEP5fjAyVHs3XWxO6IXcg0TVq7quaYqhqtRshyu28U2yt+zGp0sds/Y9ajWqVQUYVCbIzuBSBKX3ZyniAb3HFV14zQToGXGwKoRVNOg5QtmzVaoFe6kCrU+jOVxe9u9xOo0kL9k6hU5qiuxFUZ2L5jegtNCelqi5/DjxmunQIEoG6sWa4TKVv8ARk6d61r30+ZmexOxsRW3u/SiSxp5QMRVyNSR824YbobtTxLAsSeVrAaidAz6bMxAOG/ZsaVV6jlq1TMFZKyLTQmmS4UVeJIvl4C+iU8BiSK5q06BeouWmRiKmQKCcq5TR7lgb37xLdBa2hnQM+uwmY0GqZV3a0hVCVHIqGjrRU3UAqGJa5APKDVtkYqqHNVaIcvRYZMTWsUpuWWkDuQaQF75hmJN9ADpqZ0DMYbZGJQYemy0XpUcrN9NUVs4qFlNt0d4KYItcrmYXNpYbJwFZa1WtW3YzpSS1N6jA7suc9nA3dw/1ASOOpluZwgLOnToHTp06B06dOgf/9k=</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,18 +141,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,205 +491,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>slug</v>
-      </c>
-      <c r="C1" t="str">
-        <v>price</v>
-      </c>
-      <c r="D1" t="str">
-        <v>category</v>
-      </c>
-      <c r="E1" t="str">
-        <v>sellerId</v>
-      </c>
-      <c r="F1" t="str">
-        <v>shopName</v>
-      </c>
-      <c r="G1" t="str">
-        <v>images</v>
-      </c>
-      <c r="H1" t="str">
-        <v>description</v>
-      </c>
-      <c r="I1" t="str">
-        <v>stock</v>
-      </c>
-      <c r="J1" t="str">
-        <v>discount</v>
-      </c>
-      <c r="K1" t="str">
-        <v>rating</v>
-      </c>
-      <c r="L1" t="str">
-        <v>status</v>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>iPhone 15</v>
-      </c>
-      <c r="B2" t="str">
-        <v>iphone-15</v>
-      </c>
-      <c r="C2" t="str">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>5000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>4.5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
         <v>999</v>
       </c>
-      <c r="D2" t="str">
-        <v>Electronics</v>
-      </c>
-      <c r="E2" t="str">
-        <v>seller123</v>
-      </c>
-      <c r="F2" t="str">
-        <v>TechStore</v>
-      </c>
-      <c r="G2" t="str">
-        <v>https://example.com/iphone1.jpg,https://example.com/iphone2.jpg</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Latest iPhone with advanced features</v>
-      </c>
-      <c r="I2" t="str">
-        <v>50</v>
-      </c>
-      <c r="J2" t="str">
-        <v>10</v>
-      </c>
-      <c r="K2" t="str">
-        <v>4.5</v>
-      </c>
-      <c r="L2" t="str">
-        <v>active</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Samsung Galaxy S24</v>
-      </c>
-      <c r="B3" t="str">
-        <v>samsung-galaxy-s24</v>
-      </c>
-      <c r="C3" t="str">
-        <v>899</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Electronics</v>
-      </c>
-      <c r="E3" t="str">
-        <v>seller123</v>
-      </c>
-      <c r="F3" t="str">
-        <v>TechStore</v>
-      </c>
-      <c r="G3" t="str">
-        <v>https://example.com/samsung1.jpg</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Premium Android smartphone</v>
-      </c>
-      <c r="I3" t="str">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
         <v>30</v>
       </c>
-      <c r="J3" t="str">
-        <v>5</v>
-      </c>
-      <c r="K3" t="str">
-        <v>4.3</v>
-      </c>
-      <c r="L3" t="str">
-        <v>active</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Nike Air Max</v>
-      </c>
-      <c r="B4" t="str">
-        <v>nike-air-max</v>
-      </c>
-      <c r="C4" t="str">
-        <v>120</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Sports</v>
-      </c>
-      <c r="E4" t="str">
-        <v>seller456</v>
-      </c>
-      <c r="F4" t="str">
-        <v>SportsWorld</v>
-      </c>
-      <c r="G4" t="str">
-        <v>https://example.com/nike1.jpg</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Comfortable running shoes</v>
-      </c>
-      <c r="I4" t="str">
-        <v>100</v>
-      </c>
-      <c r="J4" t="str">
-        <v>15</v>
-      </c>
-      <c r="K4" t="str">
-        <v>4.7</v>
-      </c>
-      <c r="L4" t="str">
-        <v>active</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Cotton T-Shirt</v>
-      </c>
-      <c r="B5" t="str">
-        <v>cotton-t-shirt</v>
-      </c>
-      <c r="C5" t="str">
-        <v>25</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Clothing</v>
-      </c>
-      <c r="E5" t="str">
-        <v>seller789</v>
-      </c>
-      <c r="F5" t="str">
-        <v>FashionHub</v>
-      </c>
-      <c r="G5" t="str">
-        <v>https://example.com/tshirt1.jpg</v>
-      </c>
-      <c r="H5" t="str">
-        <v>100% cotton comfortable t-shirt</v>
-      </c>
-      <c r="I5" t="str">
-        <v>200</v>
-      </c>
-      <c r="J5" t="str">
-        <v>0</v>
-      </c>
-      <c r="K5" t="str">
-        <v>4.2</v>
-      </c>
-      <c r="L5" t="str">
-        <v>active</v>
+      <c r="K3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError sqref="A1:L1 D3:E3 D2:F2 L2 L3 H3 H2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>